<commit_message>
Fixed Human and Organism Subjects
</commit_message>
<xml_diff>
--- a/seronetTemplates/template/subjectAnimals.xlsx
+++ b/seronetTemplates/template/subjectAnimals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liualg/Documents/GitHub/SeroNet/seronetTemplates/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AAAD7D-99C8-6F45-94C1-F4ADC46BC89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B5279C-0384-4F40-867C-6AB2D787E98F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="20540" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20540" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="subjectAnimals.txt" sheetId="1" r:id="rId1"/>

</xml_diff>